<commit_message>
update spaMM analyses and Fig3a
122 species
</commit_message>
<xml_diff>
--- a/01_Analyses_teleo/03_Outputs/TableS3.xlsx
+++ b/01_Analyses_teleo/03_Outputs/TableS3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AliciaDalongeville\Documents\SPYGEN\CEFE\Ports_SC21250\Med_Port_eDNA\01_Analyses_teleo\03_Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BE63E04D-89CC-4CA0-A6D2-FB046883ED28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62AA4EDA-C7CB-46C8-9744-A6CC13193D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableS3" sheetId="1" r:id="rId1"/>
@@ -61,9 +61,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -561,13 +561,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -916,18 +916,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,47 +945,47 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -993,174 +993,174 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
-        <v>47.0076206103045</v>
-      </c>
-      <c r="C3" s="4">
-        <v>8.1218967280416402E-5</v>
-      </c>
-      <c r="D3" s="4">
-        <v>5.4709233076358004</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.170270412901565</v>
-      </c>
-      <c r="F3" s="4">
-        <v>8.4458466370734203E-2</v>
-      </c>
-      <c r="G3" s="4">
-        <v>0.99999592646091995</v>
-      </c>
-      <c r="H3" s="4">
-        <v>19.175788692703801</v>
-      </c>
-      <c r="I3" s="4">
-        <v>4.3444709052486998E-8</v>
+      <c r="B3" s="3">
+        <v>45.225991329705799</v>
+      </c>
+      <c r="C3" s="3">
+        <v>8.5802436945781006E-5</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4.9382488560192002</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.257871520293733</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-0.29327865257557201</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.99747374198622496</v>
+      </c>
+      <c r="H3" s="3">
+        <v>19.0501320228441</v>
+      </c>
+      <c r="I3" s="3">
+        <v>3.8335899121833001E-8</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
-        <v>10.503004069984801</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.70875887746336297</v>
-      </c>
-      <c r="D4" s="4">
-        <v>3.2299606409864099</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.51391109257084999</v>
-      </c>
-      <c r="F4" s="4">
-        <v>-4.8907360790790999E-2</v>
-      </c>
-      <c r="G4" s="4">
-        <v>0.99999942467188896</v>
-      </c>
-      <c r="H4" s="4">
-        <v>2.2873001737752001</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0.90582276762295399</v>
+      <c r="B4" s="3">
+        <v>10.7361617143558</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.68181168387547497</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3.3083541990007101</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.49797011184929102</v>
+      </c>
+      <c r="F4" s="3">
+        <v>7.2656273533539706E-2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.99999472697137404</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2.3860985335036502</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.88491135352109695</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
-        <v>-2.8761517652273501</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.88762836537775203</v>
-      </c>
-      <c r="D5" s="4">
-        <v>-2.0766589409597098</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.23804973327207901</v>
-      </c>
-      <c r="F5" s="4">
-        <v>9.1495539646150606E-2</v>
-      </c>
-      <c r="G5" s="4">
-        <v>0.99945987554418503</v>
-      </c>
-      <c r="H5" s="4">
-        <v>1.2003470281859701</v>
-      </c>
-      <c r="I5" s="4">
-        <v>0.722082548766248</v>
+      <c r="B5" s="3">
+        <v>-2.2639598437299102</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.94711971573188403</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-2.0066302442159798</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.24548357845155699</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.181296885207162</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.98645586474699698</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.32595028110463</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.63381862621239604</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4">
-        <v>-0.22302338550311501</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.99999776279030705</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.66371292111177105</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.70170025389627599</v>
-      </c>
-      <c r="F6" s="4">
-        <v>-7.85346029012816E-2</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0.98697742727141702</v>
-      </c>
-      <c r="H6" s="4">
-        <v>-0.58480614693241895</v>
-      </c>
-      <c r="I6" s="4">
-        <v>0.90694064095609095</v>
+      <c r="B6" s="3">
+        <v>-1.2296134332678E-2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.99999999999992695</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.736694583237541</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.622341988554863</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-4.99294442674907E-2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.99855347895645696</v>
+      </c>
+      <c r="H6" s="3">
+        <v>-0.54682821544475801</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.92220816336393596</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
-        <v>-2.3917668009090001</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.57202153499889796</v>
-      </c>
-      <c r="D7" s="4">
-        <v>-0.24933202134586399</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.97513530453093</v>
-      </c>
-      <c r="F7" s="4">
-        <v>4.29428195317074E-2</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0.99760166366854897</v>
-      </c>
-      <c r="H7" s="4">
-        <v>-0.83457667242755396</v>
-      </c>
-      <c r="I7" s="4">
-        <v>0.47014762439799301</v>
+      <c r="B7" s="3">
+        <v>-2.3578720565233802</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.57360907560824204</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-0.23527847328188101</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.98104625435228998</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6.7339756194770506E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.98344754986671001</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-0.87953661765325297</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.40280188186478999</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4">
-        <v>12.390913513875701</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.58110916955958603</v>
-      </c>
-      <c r="D8" s="4">
-        <v>2.6088208379248798</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.71965265075793805</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0.59136190491035101</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0.84698508323823096</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0.98028410043676595</v>
-      </c>
-      <c r="I8" s="4">
-        <v>0.99769888335453705</v>
+      <c r="B8" s="3">
+        <v>11.8429210431076</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.61048619821188399</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.6028009212968999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.72608910037894303</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.57989791005475899</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.85816164050480404</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.88062253280723901</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.998540880609184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>